<commit_message>
Created login page tests
</commit_message>
<xml_diff>
--- a/CompanyMediaTests/TestData/TestData.xlsx
+++ b/CompanyMediaTests/TestData/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\source\repos\CompanyMediaTests\CompanyMediaTests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1FCB02-93F2-49A8-A694-E5498E1A6D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B50784-E3AC-47ED-B790-0E6344CB8BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>#</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>LogIn</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>admin@localhost.com</t>
   </si>
 </sst>
 </file>
@@ -438,7 +453,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,10 +461,10 @@
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
@@ -463,10 +478,18 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -479,20 +502,26 @@
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First test in SSModule
</commit_message>
<xml_diff>
--- a/CompanyMediaTests/TestData/TestData.xlsx
+++ b/CompanyMediaTests/TestData/TestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\source\repos\CompanyMediaTests\CompanyMediaTests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F47066-4871-4538-8FE7-FF331C3CA77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0736E8CB-13BA-4CC8-BB96-59A7605718DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2655" windowWidth="24240" windowHeight="13290" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInData" sheetId="2" r:id="rId1"/>
-    <sheet name="Results" sheetId="3" r:id="rId2"/>
+    <sheet name="SystemStructureCreateData" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>25.04.2024 19:27:57</t>
-  </si>
-  <si>
-    <t>C:\Users\tomas\Documents\Reports_CianWebSiteTests_25.04.2024\DESKTOP-N2RD101_tomas_Report#8266097675955877874ZZJ4GE4_25.04.2024 19_27_57.txt</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -89,6 +83,114 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>Тип</t>
+  </si>
+  <si>
+    <t>DocProjects</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Базовый тип модуля</t>
+  </si>
+  <si>
+    <t>Комплект</t>
+  </si>
+  <si>
+    <t>Реплика</t>
+  </si>
+  <si>
+    <t>Реплика тест</t>
+  </si>
+  <si>
+    <t>Приложение протоколирования</t>
+  </si>
+  <si>
+    <t>Архив договоров</t>
+  </si>
+  <si>
+    <t>Приложение Проекты</t>
+  </si>
+  <si>
+    <t>Имя файла</t>
+  </si>
+  <si>
+    <t>Хранилище</t>
+  </si>
+  <si>
+    <t>AF5</t>
+  </si>
+  <si>
+    <t>Несистемный модуль</t>
+  </si>
+  <si>
+    <t>Именное приложение</t>
+  </si>
+  <si>
+    <t>iDocs Administrator</t>
+  </si>
+  <si>
+    <t>iDocs Storage</t>
+  </si>
+  <si>
+    <t>Locker-COK</t>
+  </si>
+  <si>
+    <t>MobileGate</t>
+  </si>
+  <si>
+    <t>Тестовое имя 1</t>
+  </si>
+  <si>
+    <t>Тестовое имя 2</t>
+  </si>
+  <si>
+    <t>Тестовое имя 3</t>
+  </si>
+  <si>
+    <t>Тестовое имя 4</t>
+  </si>
+  <si>
+    <t>Тестовое имя 5</t>
+  </si>
+  <si>
+    <t>Тест комплект 1</t>
+  </si>
+  <si>
+    <t>Тест комплект 2</t>
+  </si>
+  <si>
+    <t>Тест комплект 3</t>
+  </si>
+  <si>
+    <t>Тест комплект 4</t>
+  </si>
+  <si>
+    <t>Тест комплект 5</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Domino</t>
+  </si>
+  <si>
+    <t>Тестовое имя файла 1</t>
+  </si>
+  <si>
+    <t>Тестовое имя файла 2</t>
+  </si>
+  <si>
+    <t>Тестовое имя файла 3</t>
+  </si>
+  <si>
+    <t>Тестовое имя файла 4</t>
+  </si>
+  <si>
+    <t>Тестовое имя файла 5</t>
   </si>
 </sst>
 </file>
@@ -112,9 +214,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,9 +252,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -164,10 +263,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F855F1-CD66-4EB0-9A7C-F4C4D5989424}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -503,25 +601,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -529,23 +627,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -553,53 +651,251 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{F21DDA81-141F-45A4-8D69-175F5D1324E0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDD4775-C4E6-44E6-AC4A-03D77F1B4437}">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CreateApps test is done
</commit_message>
<xml_diff>
--- a/CompanyMediaTests/TestData/TestData.xlsx
+++ b/CompanyMediaTests/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\source\repos\CompanyMediaTests\CompanyMediaTests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0736E8CB-13BA-4CC8-BB96-59A7605718DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC0FCA6-054A-4C82-A417-DC109E959D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
+    <workbookView xWindow="-24120" yWindow="2655" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInData" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>#</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Хранилище</t>
   </si>
   <si>
-    <t>AF5</t>
-  </si>
-  <si>
     <t>Несистемный модуль</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>iDocs Storage</t>
   </si>
   <si>
-    <t>Locker-COK</t>
-  </si>
-  <si>
     <t>MobileGate</t>
   </si>
   <si>
@@ -191,6 +185,9 @@
   </si>
   <si>
     <t>Тестовое имя файла 5</t>
+  </si>
+  <si>
+    <t>Locker-СОК</t>
   </si>
 </sst>
 </file>
@@ -683,7 +680,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +709,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>19</v>
@@ -733,7 +730,7 @@
         <v>26</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>27</v>
@@ -747,25 +744,34 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
         <v>22</v>
       </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
       <c r="I2" t="s">
         <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -773,10 +779,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -785,25 +791,25 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
         <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K3" t="s">
         <v>9</v>
       </c>
       <c r="L3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -811,28 +817,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
       </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -840,28 +855,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
       </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -869,28 +893,37 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
       </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
       <c r="I6" t="s">
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>9</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created +- create and delete org's apps test
</commit_message>
<xml_diff>
--- a/CompanyMediaTests/TestData/TestData.xlsx
+++ b/CompanyMediaTests/TestData/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\source\repos\CompanyMediaTests\CompanyMediaTests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC0FCA6-054A-4C82-A417-DC109E959D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC45DB7-508F-4EE4-B914-61919898F32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2655" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
+    <workbookView xWindow="-24120" yWindow="2655" windowWidth="24240" windowHeight="13290" activeTab="2" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInData" sheetId="2" r:id="rId1"/>
     <sheet name="SystemStructureCreateData" sheetId="4" r:id="rId2"/>
+    <sheet name="SystemStructureCreateOrgsApps" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -188,6 +189,30 @@
   </si>
   <si>
     <t>Locker-СОК</t>
+  </si>
+  <si>
+    <t>Организация</t>
+  </si>
+  <si>
+    <t>Приложение</t>
+  </si>
+  <si>
+    <t>АдмГор</t>
+  </si>
+  <si>
+    <t>Тестовое имя 4ZUS6A3J</t>
+  </si>
+  <si>
+    <t>Тестовое имя 4XRVE1WJ</t>
+  </si>
+  <si>
+    <t>Тестовое имя 4XBJSER7</t>
+  </si>
+  <si>
+    <t>Тестовое имя 4VX8YZPI</t>
+  </si>
+  <si>
+    <t>Тестовое имя 4UFDZEKJ</t>
   </si>
 </sst>
 </file>
@@ -679,7 +704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDD4775-C4E6-44E6-AC4A-03D77F1B4437}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -931,4 +956,90 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9282A3B1-1BF0-4F11-93DF-33FC07839B7C}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created apps types test
</commit_message>
<xml_diff>
--- a/CompanyMediaTests/TestData/TestData.xlsx
+++ b/CompanyMediaTests/TestData/TestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\source\repos\CompanyMediaTests\CompanyMediaTests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC45DB7-508F-4EE4-B914-61919898F32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C00A580-2F82-4776-85CC-9C3BA7C42991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2655" windowWidth="24240" windowHeight="13290" activeTab="2" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInData" sheetId="2" r:id="rId1"/>
     <sheet name="SystemStructureCreateData" sheetId="4" r:id="rId2"/>
     <sheet name="SystemStructureCreateOrgsApps" sheetId="5" r:id="rId3"/>
+    <sheet name="SystemStructureCreateAppsTypes" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>#</t>
   </si>
@@ -213,6 +214,48 @@
   </si>
   <si>
     <t>Тестовое имя 4UFDZEKJ</t>
+  </si>
+  <si>
+    <t>Наименование</t>
+  </si>
+  <si>
+    <t>Идентификатор</t>
+  </si>
+  <si>
+    <t>Является корпоративным</t>
+  </si>
+  <si>
+    <t>Поддерживает работу с компонентами</t>
+  </si>
+  <si>
+    <t>Тестовое наименование 1</t>
+  </si>
+  <si>
+    <t>Тестовое наименование 2</t>
+  </si>
+  <si>
+    <t>Тестовое наименование 3</t>
+  </si>
+  <si>
+    <t>Тестовое наименование 4</t>
+  </si>
+  <si>
+    <t>Тестовое наименование 5</t>
+  </si>
+  <si>
+    <t>Тестовый идентификатор 1</t>
+  </si>
+  <si>
+    <t>Тестовый идентификатор 2</t>
+  </si>
+  <si>
+    <t>Тестовый идентификатор 3</t>
+  </si>
+  <si>
+    <t>Тестовый идентификатор 4</t>
+  </si>
+  <si>
+    <t>Тестовый идентификатор 5</t>
   </si>
 </sst>
 </file>
@@ -962,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9282A3B1-1BF0-4F11-93DF-33FC07839B7C}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1042,4 +1085,129 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A914698A-DCA0-4D47-A718-717BE5AA5B5F}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created terr create test
</commit_message>
<xml_diff>
--- a/CompanyMediaTests/TestData/TestData.xlsx
+++ b/CompanyMediaTests/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\source\repos\CompanyMediaTests\CompanyMediaTests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE7B494-6608-44F3-8AD5-2B8413E193AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606CFD1B-EA1A-4812-BEB7-7EF01FB99F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
+    <workbookView xWindow="-24120" yWindow="2655" windowWidth="24240" windowHeight="13290" firstSheet="4" activeTab="6" xr2:uid="{334D1AC5-1AD5-4C34-9CF9-5FC244EF7B18}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInData" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="SystemStructureCreateOrgsApps" sheetId="5" r:id="rId3"/>
     <sheet name="SystemStructureCreateAppsTypes" sheetId="6" r:id="rId4"/>
     <sheet name="SystemStructureCreateWSS" sheetId="7" r:id="rId5"/>
+    <sheet name="SystemStructureCreateClientApp" sheetId="8" r:id="rId6"/>
+    <sheet name="SystemStructureCreateTerr" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="126">
   <si>
     <t>#</t>
   </si>
@@ -269,13 +271,161 @@
   </si>
   <si>
     <t>Справочник персон</t>
+  </si>
+  <si>
+    <t>Тип клиентского приложения</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Def</t>
+  </si>
+  <si>
+    <t>Zxy</t>
+  </si>
+  <si>
+    <t>Центральная</t>
+  </si>
+  <si>
+    <t>Счетчик групп доступа</t>
+  </si>
+  <si>
+    <t>Префикс счётчика сети для групп доступа</t>
+  </si>
+  <si>
+    <t>Использовать часовой пояс
+Центральной территории</t>
+  </si>
+  <si>
+    <t>Часовой пояс: смещение (формат значений 03:00)</t>
+  </si>
+  <si>
+    <t>Летнее время используется</t>
+  </si>
+  <si>
+    <t>направление</t>
+  </si>
+  <si>
+    <t>Test_identifier_2109</t>
+  </si>
+  <si>
+    <t>Test_identifier_2101</t>
+  </si>
+  <si>
+    <t>Test_identifier_2102</t>
+  </si>
+  <si>
+    <t>Test_identifier_2103</t>
+  </si>
+  <si>
+    <t>Test_identifier_2104</t>
+  </si>
+  <si>
+    <t>Test_identifier_2105</t>
+  </si>
+  <si>
+    <t>Test_identifier_2106</t>
+  </si>
+  <si>
+    <t>Test_identifier_2107</t>
+  </si>
+  <si>
+    <t>Test_identifier_2108</t>
+  </si>
+  <si>
+    <t>Test_identifier_2110</t>
+  </si>
+  <si>
+    <t>Тестовое название 09</t>
+  </si>
+  <si>
+    <t>Тестовое название 10</t>
+  </si>
+  <si>
+    <t>Тестовое название 11</t>
+  </si>
+  <si>
+    <t>Тестовое название 12</t>
+  </si>
+  <si>
+    <t>Тестовое название 13</t>
+  </si>
+  <si>
+    <t>Тестовое название 14</t>
+  </si>
+  <si>
+    <t>Тестовое название 15</t>
+  </si>
+  <si>
+    <t>Тестовое название 16</t>
+  </si>
+  <si>
+    <t>Тестовое название 17</t>
+  </si>
+  <si>
+    <t>Тестовое название 18</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>d4</t>
+  </si>
+  <si>
+    <t>d5</t>
+  </si>
+  <si>
+    <t>d6</t>
+  </si>
+  <si>
+    <t>d7</t>
+  </si>
+  <si>
+    <t>d8</t>
+  </si>
+  <si>
+    <t>d9</t>
+  </si>
+  <si>
+    <t>к востоку от Гринвича</t>
+  </si>
+  <si>
+    <t>к западу от Гринвича</t>
+  </si>
+  <si>
+    <t>01:00</t>
+  </si>
+  <si>
+    <t>02:00</t>
+  </si>
+  <si>
+    <t>04:00</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>01:30</t>
+  </si>
+  <si>
+    <t>03:00</t>
+  </si>
+  <si>
+    <t>07:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +446,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -333,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -342,6 +498,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1232,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0F9A46-6CB3-4DCB-9CF9-AD8F2BFF6408}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,4 +1443,484 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A91A24A-1F8D-4857-8D93-F10522B2A90B}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9558C36-7B06-4015-AE24-5B7ADD9A5205}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" t="s">
+        <v>118</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>